<commit_message>
chore: update changes from trendyol
</commit_message>
<xml_diff>
--- a/companies/trendyol/headphoneCase/headphoneCase.xlsx
+++ b/companies/trendyol/headphoneCase/headphoneCase.xlsx
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Apple Uyumlu</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Casper</t>
+          <t>Casper Uyumlu</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>General Mobile</t>
+          <t>General Mobile Uyumlu</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Huawei Uyumlu</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>JBL</t>
+          <t>JBL Uyumlu</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>Lenovo Uyumlu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Oppo Uyumlu</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>POCO</t>
+          <t>POCO Uyumlu</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Reeder</t>
+          <t>Reeder Uyumlu</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1589,7 +1589,7 @@
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Samsung Uyumlu</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1601,7 +1601,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sennheiser</t>
+          <t>Sennheiser Uyumlu</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1613,7 +1613,7 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sony</t>
+          <t>Sony Uyumlu</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1625,7 +1625,7 @@
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Xiaomi Uyumlu</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">

</xml_diff>